<commit_message>
Ogarnąłem te pliki do końca bo czasami nie były sformatowane dobrze i wczytałem je jako data frame pandasowe
</commit_message>
<xml_diff>
--- a/Data/companies_with most_autonomus_drivin_patensts.xlsx
+++ b/Data/companies_with most_autonomus_drivin_patensts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Continental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUM</t>
   </si>
   <si>
     <t xml:space="preserve">2010</t>
@@ -95,6 +98,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -206,10 +210,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -248,10 +252,13 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>621</v>
@@ -280,10 +287,14 @@
       <c r="J2" s="4" t="n">
         <v>199</v>
       </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">SUM(B2:J2)</f>
+        <v>2209</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>683</v>
@@ -312,10 +323,14 @@
       <c r="J3" s="4" t="n">
         <v>224</v>
       </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">SUM(B3:J3)</f>
+        <v>2449</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>745</v>
@@ -344,10 +359,14 @@
       <c r="J4" s="4" t="n">
         <v>247</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">SUM(B4:J4)</f>
+        <v>2718</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>809</v>
@@ -376,10 +395,14 @@
       <c r="J5" s="4" t="n">
         <v>283</v>
       </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">SUM(B5:J5)</f>
+        <v>3186</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>875</v>
@@ -408,10 +431,14 @@
       <c r="J6" s="4" t="n">
         <v>331</v>
       </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">SUM(B6:J6)</f>
+        <v>3699</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>946</v>
@@ -440,10 +467,14 @@
       <c r="J7" s="4" t="n">
         <v>392</v>
       </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">SUM(B7:J7)</f>
+        <v>4406</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>1134</v>
@@ -472,10 +503,14 @@
       <c r="J8" s="4" t="n">
         <v>480</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">SUM(B8:J8)</f>
+        <v>5471</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>1325</v>
@@ -504,10 +539,14 @@
       <c r="J9" s="4" t="n">
         <v>560</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <f aca="false">SUM(B9:J9)</f>
+        <v>6873</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>1668</v>
@@ -536,10 +575,14 @@
       <c r="J10" s="4" t="n">
         <v>653</v>
       </c>
+      <c r="K10" s="0" t="n">
+        <f aca="false">SUM(B10:J10)</f>
+        <v>8948</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>1756</v>
@@ -567,6 +610,10 @@
       </c>
       <c r="J11" s="4" t="n">
         <v>689</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <f aca="false">SUM(B11:J11)</f>
+        <v>9487</v>
       </c>
     </row>
   </sheetData>

</xml_diff>